<commit_message>
feat(commands): adapt xlspython to the new MVC architecture
</commit_message>
<xml_diff>
--- a/fichiers_xls/gathertests/Nouveau dossier - Copie/jouet.xlsx
+++ b/fichiers_xls/gathertests/Nouveau dossier - Copie/jouet.xlsx
@@ -770,7 +770,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
@@ -781,378 +781,168 @@
     <row r="1" ht="12.75" customHeight="1" s="6">
       <c r="A1" s="7" t="inlineStr">
         <is>
-          <t>Prénom</t>
+          <t>Temps utilisé</t>
         </is>
       </c>
       <c r="B1" s="7" t="inlineStr">
         <is>
-          <t>État</t>
-        </is>
-      </c>
-      <c r="C1" s="7" t="inlineStr">
-        <is>
-          <t>Temps utilisé</t>
-        </is>
-      </c>
-      <c r="D1" s="7" t="inlineStr">
-        <is>
           <t>Note/10,00</t>
         </is>
       </c>
-      <c r="E1" s="7" t="inlineStr">
-        <is>
-          <t>Réponse 1</t>
-        </is>
-      </c>
     </row>
     <row r="2" ht="12.75" customHeight="1" s="6">
-      <c r="A2" s="7" t="inlineStr">
-        <is>
-          <t>Paola</t>
+      <c r="A2" s="8" t="inlineStr">
+        <is>
+          <t>8 min 33 s</t>
         </is>
       </c>
       <c r="B2" s="7" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="C2" s="8" t="inlineStr">
-        <is>
-          <t>8 min 33 s</t>
-        </is>
-      </c>
-      <c r="D2" s="7" t="inlineStr">
-        <is>
           <t>7,16</t>
         </is>
       </c>
-      <c r="E2" s="7" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="6">
-      <c r="A3" s="7" t="inlineStr">
-        <is>
-          <t>Zina</t>
+      <c r="A3" s="8" t="inlineStr">
+        <is>
+          <t>5 min 15 s</t>
         </is>
       </c>
       <c r="B3" s="7" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="C3" s="8" t="inlineStr">
-        <is>
-          <t>5 min 15 s</t>
-        </is>
-      </c>
-      <c r="D3" s="7" t="inlineStr">
-        <is>
           <t>7,28</t>
         </is>
       </c>
-      <c r="E3" s="7" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="6">
-      <c r="A4" s="7" t="inlineStr">
-        <is>
-          <t>Aboubaker</t>
+      <c r="A4" s="8" t="inlineStr">
+        <is>
+          <t>7 min 57 s</t>
         </is>
       </c>
       <c r="B4" s="7" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="C4" s="8" t="inlineStr">
-        <is>
-          <t>7 min 57 s</t>
-        </is>
-      </c>
-      <c r="D4" s="7" t="inlineStr">
-        <is>
           <t>7,98</t>
         </is>
       </c>
-      <c r="E4" s="7" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="6">
-      <c r="A5" s="7" t="inlineStr">
-        <is>
-          <t>Yasmine</t>
+      <c r="A5" s="8" t="inlineStr">
+        <is>
+          <t>7 min 22 s</t>
         </is>
       </c>
       <c r="B5" s="7" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="C5" s="8" t="inlineStr">
-        <is>
-          <t>7 min 22 s</t>
-        </is>
-      </c>
-      <c r="D5" s="7" t="inlineStr">
-        <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="E5" s="7" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
     </row>
     <row r="6" ht="12.75" customHeight="1" s="6">
-      <c r="A6" s="7" t="inlineStr">
-        <is>
-          <t>Yasmine</t>
+      <c r="A6" s="8" t="inlineStr">
+        <is>
+          <t>7 min 44 s</t>
         </is>
       </c>
       <c r="B6" s="7" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="C6" s="8" t="inlineStr">
-        <is>
-          <t>7 min 44 s</t>
-        </is>
-      </c>
-      <c r="D6" s="7" t="inlineStr">
-        <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="E6" s="7" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="6">
-      <c r="A7" s="7" t="inlineStr">
-        <is>
-          <t>Hassan Mahamat</t>
+      <c r="A7" s="9" t="inlineStr">
+        <is>
+          <t>23 min 37 s</t>
         </is>
       </c>
       <c r="B7" s="7" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="C7" s="9" t="inlineStr">
-        <is>
-          <t>23 min 37 s</t>
-        </is>
-      </c>
-      <c r="D7" s="7" t="inlineStr">
-        <is>
           <t>7,52</t>
         </is>
       </c>
-      <c r="E7" s="7" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
     </row>
     <row r="8" ht="12.75" customHeight="1" s="6">
-      <c r="A8" s="7" t="inlineStr">
-        <is>
-          <t>Nouh</t>
+      <c r="A8" s="8" t="inlineStr">
+        <is>
+          <t>9 min 27 s</t>
         </is>
       </c>
       <c r="B8" s="7" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="C8" s="8" t="inlineStr">
-        <is>
-          <t>9 min 27 s</t>
-        </is>
-      </c>
-      <c r="D8" s="7" t="inlineStr">
-        <is>
           <t>7,35</t>
         </is>
       </c>
-      <c r="E8" s="7" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
     </row>
     <row r="9" ht="12.75" customHeight="1" s="6">
-      <c r="A9" s="7" t="inlineStr">
-        <is>
-          <t>Yacine</t>
+      <c r="A9" s="8" t="inlineStr">
+        <is>
+          <t>4 min 17 s</t>
         </is>
       </c>
       <c r="B9" s="7" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>4 min 17 s</t>
-        </is>
-      </c>
-      <c r="D9" s="7" t="inlineStr">
-        <is>
           <t>8,07</t>
         </is>
       </c>
-      <c r="E9" s="7" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
     </row>
     <row r="10" ht="12.75" customHeight="1" s="6">
-      <c r="A10" s="7" t="inlineStr">
-        <is>
-          <t>Iness</t>
+      <c r="A10" s="8" t="inlineStr">
+        <is>
+          <t>10 min 33 s</t>
         </is>
       </c>
       <c r="B10" s="7" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="C10" s="8" t="inlineStr">
-        <is>
-          <t>10 min 33 s</t>
-        </is>
-      </c>
-      <c r="D10" s="7" t="inlineStr">
-        <is>
           <t>6,51</t>
         </is>
       </c>
-      <c r="E10" s="7" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
     </row>
     <row r="11" ht="12.75" customHeight="1" s="6">
-      <c r="A11" s="7" t="inlineStr">
-        <is>
-          <t>Houzefa</t>
+      <c r="A11" s="8" t="inlineStr">
+        <is>
+          <t>5 min 49 s</t>
         </is>
       </c>
       <c r="B11" s="7" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="C11" s="8" t="inlineStr">
-        <is>
-          <t>5 min 49 s</t>
-        </is>
-      </c>
-      <c r="D11" s="7" t="inlineStr">
-        <is>
           <t>7,83</t>
         </is>
       </c>
-      <c r="E11" s="7" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
     </row>
     <row r="12" ht="12.75" customHeight="1" s="6">
-      <c r="A12" s="7" t="inlineStr">
-        <is>
-          <t>Zakaria</t>
+      <c r="A12" s="8" t="inlineStr">
+        <is>
+          <t>9 min 14 s</t>
         </is>
       </c>
       <c r="B12" s="7" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="C12" s="8" t="inlineStr">
-        <is>
-          <t>9 min 14 s</t>
-        </is>
-      </c>
-      <c r="D12" s="7" t="inlineStr">
-        <is>
           <t>7,70</t>
         </is>
       </c>
-      <c r="E12" s="7" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
     </row>
     <row r="13" ht="12.75" customHeight="1" s="6">
-      <c r="A13" s="10" t="inlineStr">
-        <is>
-          <t>Rodolphe</t>
+      <c r="A13" s="8" t="inlineStr">
+        <is>
+          <t>15 min 32 s</t>
         </is>
       </c>
       <c r="B13" s="7" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="C13" s="8" t="inlineStr">
-        <is>
-          <t>15 min 32 s</t>
-        </is>
-      </c>
-      <c r="D13" s="7" t="inlineStr">
-        <is>
           <t>8,88</t>
         </is>
       </c>
-      <c r="E13" s="7" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
-        </is>
-      </c>
     </row>
     <row r="14" ht="12.75" customHeight="1" s="6">
-      <c r="A14" s="10" t="inlineStr">
-        <is>
-          <t>Christian</t>
+      <c r="A14" s="9" t="inlineStr">
+        <is>
+          <t>21 min 49 s</t>
         </is>
       </c>
       <c r="B14" s="7" t="inlineStr">
         <is>
-          <t>Terminé</t>
-        </is>
-      </c>
-      <c r="C14" s="9" t="inlineStr">
-        <is>
-          <t>21 min 49 s</t>
-        </is>
-      </c>
-      <c r="D14" s="7" t="inlineStr">
-        <is>
           <t>6,72</t>
-        </is>
-      </c>
-      <c r="E14" s="7" t="inlineStr">
-        <is>
-          <t>Je suis d’accord pour que mes réponses soient exploitées à des fins de recherche</t>
         </is>
       </c>
     </row>

</xml_diff>